<commit_message>
Add files to export data from openBIS to Excel, to create a flatten version of JSON-LD, and to import/export the entire database from openBIS account
</commit_message>
<xml_diff>
--- a/Metadata_Experiment_Objects.xlsx
+++ b/Metadata_Experiment_Objects.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dafa\Documents\git\nanotech-premise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dafa\Documents\git\metadata-spectroscopy\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12045"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiment" sheetId="11" r:id="rId1"/>
+    <sheet name="Relations" sheetId="11" r:id="rId1"/>
     <sheet name="Supplier" sheetId="45" r:id="rId2"/>
     <sheet name="Room" sheetId="47" r:id="rId3"/>
     <sheet name="Manufacturer" sheetId="46" r:id="rId4"/>
@@ -1260,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>

</xml_diff>